<commit_message>
Phân quyền trang danh sách hộ cá thể + fix bug
</commit_message>
<xml_diff>
--- a/TelerikWebApp1/DanhSachHoCaThe_Import (1).xlsx
+++ b/TelerikWebApp1/DanhSachHoCaThe_Import (1).xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Mã số thuế</t>
   </si>
@@ -115,28 +110,19 @@
     <t>XV</t>
   </si>
   <si>
-    <t>sadsad</t>
-  </si>
-  <si>
-    <t>27/1/1988</t>
-  </si>
-  <si>
-    <t>hrwjhrew</t>
-  </si>
-  <si>
-    <t>dđsfdf</t>
-  </si>
-  <si>
-    <t>vcnvmcvn</t>
-  </si>
-  <si>
-    <t>22/6/2018</t>
+    <t>LÊ GIA HUY</t>
+  </si>
+  <si>
+    <t>15/12/2018</t>
+  </si>
+  <si>
+    <t>bán muối</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -497,16 +483,16 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,11 +523,8 @@
       <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -572,46 +555,32 @@
       <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>1234643</v>
+        <v>123456789</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="6">
-        <v>231321321</v>
+        <v>25471122</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="6">
-        <v>232372</v>
-      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
       <c r="J3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -622,11 +591,8 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="P4" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -637,11 +603,8 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="P5" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -652,11 +615,8 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="P6" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -667,11 +627,8 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="P7" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -682,11 +639,8 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="P8" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -697,11 +651,8 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="P9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -712,11 +663,8 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="P10" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -728,7 +676,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -740,7 +688,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -752,7 +700,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -764,7 +712,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -776,7 +724,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -788,7 +736,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -800,7 +748,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -812,7 +760,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -823,8 +771,11 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P19" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -835,8 +786,11 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P20" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -847,8 +801,11 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P21" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -859,8 +816,11 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P22" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -871,8 +831,11 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P23" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -883,8 +846,11 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -895,8 +861,11 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P25" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -907,8 +876,11 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P26" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -919,8 +891,11 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P27" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -931,8 +906,11 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="P28" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -944,7 +922,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -956,7 +934,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -968,7 +946,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -980,7 +958,7 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -992,7 +970,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1004,7 +982,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1016,7 +994,7 @@
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1028,7 +1006,7 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1040,7 +1018,7 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1052,7 +1030,7 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1064,7 +1042,7 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1076,7 +1054,7 @@
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1088,7 +1066,7 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1100,7 +1078,7 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1112,7 +1090,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1124,7 +1102,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1136,7 +1114,7 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1148,7 +1126,7 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1160,7 +1138,7 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1172,7 +1150,7 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1184,7 +1162,7 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1199,7 +1177,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J50">
-      <formula1>$P$1:$P$10</formula1>
+      <formula1>$P$19:$P$28</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1212,7 +1190,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1224,7 +1202,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>